<commit_message>
Prestes a fazer merda
</commit_message>
<xml_diff>
--- a/contatos_checados.xlsx
+++ b/contatos_checados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,10 +466,17 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>966652864</v>
+        <v>990033942</v>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>966652864</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>